<commit_message>
Fix de Analisis de Market Basket
</commit_message>
<xml_diff>
--- a/data/cedis_clasificacion_abc_ponderada.xlsx
+++ b/data/cedis_clasificacion_abc_ponderada.xlsx
@@ -981,7 +981,7 @@
         <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8">
         <v>0.005952380952380952</v>
@@ -2062,7 +2062,7 @@
         <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31">
         <v>0.001428571428571429</v>
@@ -2109,7 +2109,7 @@
         <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F32">
         <v>0.002314814814814815</v>
@@ -2814,7 +2814,7 @@
         <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F47">
         <v>0.003571428571428571</v>
@@ -3143,7 +3143,7 @@
         <v>47</v>
       </c>
       <c r="D54" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F54">
         <v>0.001041666666666667</v>

</xml_diff>